<commit_message>
Updated ui claims data
</commit_message>
<xml_diff>
--- a/data/ui_claims.xlsx
+++ b/data/ui_claims.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/Projects/ui-explainer/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malcalakovalski\Documents\Projects\ui-explainer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FC3743-3A4C-EA43-85C9-6B89B4E5B3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C7E3C7-4F76-4D36-9244-F74E67C66C2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19760" xr2:uid="{5BA5F702-7B72-47BE-A4B7-F1D3AD03D02D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5BA5F702-7B72-47BE-A4B7-F1D3AD03D02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_DLX1.USE">Sheet1!$A$1:$K$4</definedName>
+    <definedName name="_DLX2.USE">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="144">
   <si>
     <t>LIUTP@WEEKLY</t>
   </si>
@@ -414,6 +416,60 @@
   </si>
   <si>
     <t>stc_workshare</t>
+  </si>
+  <si>
+    <t>2021-Oct-09W</t>
+  </si>
+  <si>
+    <t>2021-Oct-16W</t>
+  </si>
+  <si>
+    <t>2021-Oct-23W</t>
+  </si>
+  <si>
+    <t>2021-Oct-30W</t>
+  </si>
+  <si>
+    <t>2021-Nov-06W</t>
+  </si>
+  <si>
+    <t>2021-Nov-13W</t>
+  </si>
+  <si>
+    <t>2021-Nov-20W</t>
+  </si>
+  <si>
+    <t>2021-Nov-27W</t>
+  </si>
+  <si>
+    <t>2021-Dec-04W</t>
+  </si>
+  <si>
+    <t>2021-Dec-11W</t>
+  </si>
+  <si>
+    <t>2021-Dec-18W</t>
+  </si>
+  <si>
+    <t>2021-Dec-25W</t>
+  </si>
+  <si>
+    <t>2022-Jan-01W</t>
+  </si>
+  <si>
+    <t>2022-Jan-08W</t>
+  </si>
+  <si>
+    <t>2022-Jan-15W</t>
+  </si>
+  <si>
+    <t>2022-Jan-22W</t>
+  </si>
+  <si>
+    <t>2022-Jan-29W</t>
+  </si>
+  <si>
+    <t>2022-Feb-05W</t>
   </si>
 </sst>
 </file>
@@ -767,27 +823,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23B3C30-ACCF-455C-A20C-4B55670D97FF}">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="J1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="64" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.36328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -819,7 +875,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -851,7 +907,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -883,7 +939,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -915,7 +971,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -947,7 +1003,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -979,7 +1035,7 @@
         <v>10176</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1011,7 +1067,7 @@
         <v>11839</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1043,7 +1099,7 @@
         <v>10726</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1075,7 +1131,7 @@
         <v>13220</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1107,7 +1163,7 @@
         <v>11329</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1139,7 +1195,7 @@
         <v>13509</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1171,7 +1227,7 @@
         <v>13077</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1203,7 +1259,7 @@
         <v>13986</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1235,7 +1291,7 @@
         <v>11564</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1267,7 +1323,7 @@
         <v>12354</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1299,7 +1355,7 @@
         <v>12886</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1331,7 +1387,7 @@
         <v>16427</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1363,7 +1419,7 @@
         <v>25914</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1395,7 +1451,7 @@
         <v>39863</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1427,7 +1483,7 @@
         <v>62328</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1459,7 +1515,7 @@
         <v>88770</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1491,7 +1547,7 @@
         <v>122675</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1523,7 +1579,7 @@
         <v>143441</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1555,7 +1611,7 @@
         <v>179659</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1587,7 +1643,7 @@
         <v>194825</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1619,7 +1675,7 @@
         <v>214889</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1651,7 +1707,7 @@
         <v>228733</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1683,7 +1739,7 @@
         <v>292984</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1715,7 +1771,7 @@
         <v>305738</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1747,7 +1803,7 @@
         <v>361593</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -1779,7 +1835,7 @@
         <v>343559</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1811,7 +1867,7 @@
         <v>440708</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1843,7 +1899,7 @@
         <v>398908</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1875,7 +1931,7 @@
         <v>413385</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -1907,7 +1963,7 @@
         <v>451485</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -1939,7 +1995,7 @@
         <v>316243</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -1971,7 +2027,7 @@
         <v>304861</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>56</v>
       </c>
@@ -2003,7 +2059,7 @@
         <v>270232</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>57</v>
       </c>
@@ -2035,7 +2091,7 @@
         <v>253431</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2067,7 +2123,7 @@
         <v>240083</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -2099,7 +2155,7 @@
         <v>220538</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>60</v>
       </c>
@@ -2131,7 +2187,7 @@
         <v>212198</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>61</v>
       </c>
@@ -2163,7 +2219,7 @@
         <v>209661</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>62</v>
       </c>
@@ -2195,7 +2251,7 @@
         <v>196528</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -2227,7 +2283,7 @@
         <v>195366</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>64</v>
       </c>
@@ -2259,7 +2315,7 @@
         <v>187008</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -2291,7 +2347,7 @@
         <v>178444</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>66</v>
       </c>
@@ -2323,7 +2379,7 @@
         <v>163962</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -2355,7 +2411,7 @@
         <v>144395</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>68</v>
       </c>
@@ -2387,7 +2443,7 @@
         <v>128819</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>69</v>
       </c>
@@ -2419,7 +2475,7 @@
         <v>125389</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>70</v>
       </c>
@@ -2451,7 +2507,7 @@
         <v>101267</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>71</v>
       </c>
@@ -2483,7 +2539,7 @@
         <v>111061</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>72</v>
       </c>
@@ -2515,7 +2571,7 @@
         <v>99255</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>73</v>
       </c>
@@ -2547,7 +2603,7 @@
         <v>105307</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>74</v>
       </c>
@@ -2579,7 +2635,7 @@
         <v>91221</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>75</v>
       </c>
@@ -2611,7 +2667,7 @@
         <v>94819</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -2643,7 +2699,7 @@
         <v>86498</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>77</v>
       </c>
@@ -2675,7 +2731,7 @@
         <v>102571</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -2707,7 +2763,7 @@
         <v>94293</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -2739,7 +2795,7 @@
         <v>102592</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>80</v>
       </c>
@@ -2771,7 +2827,7 @@
         <v>104342</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>81</v>
       </c>
@@ -2803,7 +2859,7 @@
         <v>105587</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -2835,7 +2891,7 @@
         <v>102200</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>83</v>
       </c>
@@ -2867,7 +2923,7 @@
         <v>114736</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>84</v>
       </c>
@@ -2899,7 +2955,7 @@
         <v>103776</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>85</v>
       </c>
@@ -2931,7 +2987,7 @@
         <v>109765</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>86</v>
       </c>
@@ -2963,7 +3019,7 @@
         <v>102500</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>87</v>
       </c>
@@ -2995,7 +3051,7 @@
         <v>95695</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -3027,7 +3083,7 @@
         <v>83864</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>89</v>
       </c>
@@ -3059,7 +3115,7 @@
         <v>84983</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>90</v>
       </c>
@@ -3091,7 +3147,7 @@
         <v>83340</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>91</v>
       </c>
@@ -3123,7 +3179,7 @@
         <v>88222</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>92</v>
       </c>
@@ -3155,7 +3211,7 @@
         <v>82219</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>93</v>
       </c>
@@ -3187,7 +3243,7 @@
         <v>80286</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>94</v>
       </c>
@@ -3219,7 +3275,7 @@
         <v>84856</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>95</v>
       </c>
@@ -3251,7 +3307,7 @@
         <v>86664</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>96</v>
       </c>
@@ -3283,7 +3339,7 @@
         <v>88969</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>97</v>
       </c>
@@ -3315,7 +3371,7 @@
         <v>80239</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>98</v>
       </c>
@@ -3347,7 +3403,7 @@
         <v>83235</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>99</v>
       </c>
@@ -3379,7 +3435,7 @@
         <v>81750</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>100</v>
       </c>
@@ -3411,7 +3467,7 @@
         <v>77112</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>101</v>
       </c>
@@ -3443,7 +3499,7 @@
         <v>75157</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>102</v>
       </c>
@@ -3475,7 +3531,7 @@
         <v>64079</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>103</v>
       </c>
@@ -3507,7 +3563,7 @@
         <v>55154</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>104</v>
       </c>
@@ -3539,7 +3595,7 @@
         <v>55345</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>105</v>
       </c>
@@ -3571,7 +3627,7 @@
         <v>50681</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>106</v>
       </c>
@@ -3603,7 +3659,7 @@
         <v>47813</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>107</v>
       </c>
@@ -3635,7 +3691,7 @@
         <v>45843</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>108</v>
       </c>
@@ -3667,7 +3723,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>109</v>
       </c>
@@ -3699,7 +3755,7 @@
         <v>42694</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>110</v>
       </c>
@@ -3731,7 +3787,7 @@
         <v>42382</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>111</v>
       </c>
@@ -3763,7 +3819,7 @@
         <v>40860</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>112</v>
       </c>
@@ -3795,7 +3851,7 @@
         <v>28762</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>113</v>
       </c>
@@ -3827,7 +3883,7 @@
         <v>24231</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>114</v>
       </c>
@@ -3859,15 +3915,15 @@
         <v>23431</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>115</v>
       </c>
       <c r="B97" s="2">
-        <v>3279036</v>
+        <v>3279047</v>
       </c>
       <c r="C97" s="2">
-        <v>2255908</v>
+        <v>2255919</v>
       </c>
       <c r="D97" s="2">
         <v>7682</v>
@@ -3889,9 +3945,599 @@
       </c>
       <c r="J97" s="2">
         <v>23189</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>126</v>
+      </c>
+      <c r="B98" s="2">
+        <v>2830679</v>
+      </c>
+      <c r="C98" s="2">
+        <v>2161098</v>
+      </c>
+      <c r="D98" s="2">
+        <v>7712</v>
+      </c>
+      <c r="E98" s="2">
+        <v>5203</v>
+      </c>
+      <c r="F98" s="2">
+        <v>270013</v>
+      </c>
+      <c r="G98" s="2">
+        <v>244379</v>
+      </c>
+      <c r="H98" s="2">
+        <v>117559</v>
+      </c>
+      <c r="I98" s="2">
+        <v>2445</v>
+      </c>
+      <c r="J98" s="2">
+        <v>22270</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>127</v>
+      </c>
+      <c r="B99" s="2">
+        <v>2672948</v>
+      </c>
+      <c r="C99" s="2">
+        <v>1980615</v>
+      </c>
+      <c r="D99" s="2">
+        <v>7985</v>
+      </c>
+      <c r="E99" s="2">
+        <v>5428</v>
+      </c>
+      <c r="F99" s="2">
+        <v>277109</v>
+      </c>
+      <c r="G99" s="2">
+        <v>233684</v>
+      </c>
+      <c r="H99" s="2">
+        <v>144319</v>
+      </c>
+      <c r="I99" s="2">
+        <v>2933</v>
+      </c>
+      <c r="J99" s="2">
+        <v>20875</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>128</v>
+      </c>
+      <c r="B100" s="2">
+        <v>2565853</v>
+      </c>
+      <c r="C100" s="2">
+        <v>1878195</v>
+      </c>
+      <c r="D100" s="2">
+        <v>7927</v>
+      </c>
+      <c r="E100" s="2">
+        <v>5047</v>
+      </c>
+      <c r="F100" s="2">
+        <v>253593</v>
+      </c>
+      <c r="G100" s="2">
+        <v>256496</v>
+      </c>
+      <c r="H100" s="2">
+        <v>140150</v>
+      </c>
+      <c r="I100" s="2">
+        <v>2444</v>
+      </c>
+      <c r="J100" s="2">
+        <v>22001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>129</v>
+      </c>
+      <c r="B101" s="2">
+        <v>2608345</v>
+      </c>
+      <c r="C101" s="2">
+        <v>1946301</v>
+      </c>
+      <c r="D101" s="2">
+        <v>8023</v>
+      </c>
+      <c r="E101" s="2">
+        <v>5001</v>
+      </c>
+      <c r="F101" s="2">
+        <v>214734</v>
+      </c>
+      <c r="G101" s="2">
+        <v>272974</v>
+      </c>
+      <c r="H101" s="2">
+        <v>136208</v>
+      </c>
+      <c r="I101" s="2">
+        <v>3172</v>
+      </c>
+      <c r="J101" s="2">
+        <v>21932</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>130</v>
+      </c>
+      <c r="B102" s="2">
+        <v>2284789</v>
+      </c>
+      <c r="C102" s="2">
+        <v>1778063</v>
+      </c>
+      <c r="D102" s="2">
+        <v>7854</v>
+      </c>
+      <c r="E102" s="2">
+        <v>4837</v>
+      </c>
+      <c r="F102" s="2">
+        <v>187243</v>
+      </c>
+      <c r="G102" s="2">
+        <v>151556</v>
+      </c>
+      <c r="H102" s="2">
+        <v>134116</v>
+      </c>
+      <c r="I102" s="2">
+        <v>2985</v>
+      </c>
+      <c r="J102" s="2">
+        <v>18135</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>131</v>
+      </c>
+      <c r="B103" s="2">
+        <v>2298125</v>
+      </c>
+      <c r="C103" s="2">
+        <v>1815613</v>
+      </c>
+      <c r="D103" s="2">
+        <v>8511</v>
+      </c>
+      <c r="E103" s="2">
+        <v>5086</v>
+      </c>
+      <c r="F103" s="2">
+        <v>170300</v>
+      </c>
+      <c r="G103" s="2">
+        <v>146449</v>
+      </c>
+      <c r="H103" s="2">
+        <v>131403</v>
+      </c>
+      <c r="I103" s="2">
+        <v>2855</v>
+      </c>
+      <c r="J103" s="2">
+        <v>17908</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>132</v>
+      </c>
+      <c r="B104" s="2">
+        <v>1947611</v>
+      </c>
+      <c r="C104" s="2">
+        <v>1557232</v>
+      </c>
+      <c r="D104" s="2">
+        <v>7950</v>
+      </c>
+      <c r="E104" s="2">
+        <v>4300</v>
+      </c>
+      <c r="F104" s="2">
+        <v>124536</v>
+      </c>
+      <c r="G104" s="2">
+        <v>112728</v>
+      </c>
+      <c r="H104" s="2">
+        <v>124145</v>
+      </c>
+      <c r="I104" s="2">
+        <v>2082</v>
+      </c>
+      <c r="J104" s="2">
+        <v>14638</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>133</v>
+      </c>
+      <c r="B105" s="2">
+        <v>2458432</v>
+      </c>
+      <c r="C105" s="2">
+        <v>1960392</v>
+      </c>
+      <c r="D105" s="2">
+        <v>9786</v>
+      </c>
+      <c r="E105" s="2">
+        <v>5301</v>
+      </c>
+      <c r="F105" s="2">
+        <v>194189</v>
+      </c>
+      <c r="G105" s="2">
+        <v>136413</v>
+      </c>
+      <c r="H105" s="2">
+        <v>132622</v>
+      </c>
+      <c r="I105" s="2">
+        <v>2630</v>
+      </c>
+      <c r="J105" s="2">
+        <v>17099</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>134</v>
+      </c>
+      <c r="B106" s="2">
+        <v>2137992</v>
+      </c>
+      <c r="C106" s="2">
+        <v>1729956</v>
+      </c>
+      <c r="D106" s="2">
+        <v>9824</v>
+      </c>
+      <c r="E106" s="2">
+        <v>4718</v>
+      </c>
+      <c r="F106" s="2">
+        <v>133763</v>
+      </c>
+      <c r="G106" s="2">
+        <v>116434</v>
+      </c>
+      <c r="H106" s="2">
+        <v>124276</v>
+      </c>
+      <c r="I106" s="2">
+        <v>2252</v>
+      </c>
+      <c r="J106" s="2">
+        <v>16769</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>135</v>
+      </c>
+      <c r="B107" s="2">
+        <v>1922221</v>
+      </c>
+      <c r="C107" s="2">
+        <v>1823515</v>
+      </c>
+      <c r="D107" s="2">
+        <v>9465</v>
+      </c>
+      <c r="E107" s="2">
+        <v>4764</v>
+      </c>
+      <c r="F107" s="2">
+        <v>137421</v>
+      </c>
+      <c r="G107" s="2">
+        <v>117721</v>
+      </c>
+      <c r="H107" s="2">
+        <v>67543</v>
+      </c>
+      <c r="I107" s="2">
+        <v>2434</v>
+      </c>
+      <c r="J107" s="2">
+        <v>14500</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>136</v>
+      </c>
+      <c r="B108" s="2">
+        <v>1722360</v>
+      </c>
+      <c r="C108" s="2">
+        <v>1634510</v>
+      </c>
+      <c r="D108" s="2">
+        <v>9422</v>
+      </c>
+      <c r="E108" s="2">
+        <v>4236</v>
+      </c>
+      <c r="F108" s="2">
+        <v>91879</v>
+      </c>
+      <c r="G108" s="2">
+        <v>99163</v>
+      </c>
+      <c r="H108" s="2">
+        <v>57674</v>
+      </c>
+      <c r="I108" s="2">
+        <v>2186</v>
+      </c>
+      <c r="J108" s="2">
+        <v>14332</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>137</v>
+      </c>
+      <c r="B109" s="2">
+        <v>1948638</v>
+      </c>
+      <c r="C109" s="2">
+        <v>1865443</v>
+      </c>
+      <c r="D109" s="2">
+        <v>9619</v>
+      </c>
+      <c r="E109" s="2">
+        <v>4551</v>
+      </c>
+      <c r="F109" s="2">
+        <v>97425</v>
+      </c>
+      <c r="G109" s="2">
+        <v>47670</v>
+      </c>
+      <c r="H109" s="2">
+        <v>53633</v>
+      </c>
+      <c r="I109" s="2">
+        <v>1999</v>
+      </c>
+      <c r="J109" s="2">
+        <v>13393</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>138</v>
+      </c>
+      <c r="B110" s="2">
+        <v>2132542</v>
+      </c>
+      <c r="C110" s="2">
+        <v>2048131</v>
+      </c>
+      <c r="D110" s="2">
+        <v>10661</v>
+      </c>
+      <c r="E110" s="2">
+        <v>4765</v>
+      </c>
+      <c r="F110" s="2">
+        <v>107338</v>
+      </c>
+      <c r="G110" s="2">
+        <v>60607</v>
+      </c>
+      <c r="H110" s="2">
+        <v>52532</v>
+      </c>
+      <c r="I110" s="2">
+        <v>1991</v>
+      </c>
+      <c r="J110" s="2">
+        <v>14462</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>139</v>
+      </c>
+      <c r="B111" s="2">
+        <v>2140986</v>
+      </c>
+      <c r="C111" s="2">
+        <v>2060087</v>
+      </c>
+      <c r="D111" s="2">
+        <v>10130</v>
+      </c>
+      <c r="E111" s="2">
+        <v>5046</v>
+      </c>
+      <c r="F111" s="2">
+        <v>108321</v>
+      </c>
+      <c r="G111" s="2">
+        <v>59407</v>
+      </c>
+      <c r="H111" s="2">
+        <v>48096</v>
+      </c>
+      <c r="I111" s="2">
+        <v>2167</v>
+      </c>
+      <c r="J111" s="2">
+        <v>15460</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>140</v>
+      </c>
+      <c r="B112" s="2">
+        <v>2067788</v>
+      </c>
+      <c r="C112" s="2">
+        <v>1996633</v>
+      </c>
+      <c r="D112" s="2">
+        <v>10911</v>
+      </c>
+      <c r="E112" s="2">
+        <v>4714</v>
+      </c>
+      <c r="F112" s="2">
+        <v>77841</v>
+      </c>
+      <c r="G112" s="2">
+        <v>50338</v>
+      </c>
+      <c r="H112" s="2">
+        <v>38085</v>
+      </c>
+      <c r="I112" s="2">
+        <v>2170</v>
+      </c>
+      <c r="J112" s="2">
+        <v>15275</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113" s="2">
+        <v>2099862</v>
+      </c>
+      <c r="C113" s="2">
+        <v>2029981</v>
+      </c>
+      <c r="D113" s="2">
+        <v>10528</v>
+      </c>
+      <c r="E113" s="2">
+        <v>5088</v>
+      </c>
+      <c r="F113" s="2">
+        <v>82650</v>
+      </c>
+      <c r="G113" s="2">
+        <v>54178</v>
+      </c>
+      <c r="H113" s="2">
+        <v>36539</v>
+      </c>
+      <c r="I113" s="2">
+        <v>2251</v>
+      </c>
+      <c r="J113" s="2">
+        <v>15475</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>142</v>
+      </c>
+      <c r="B114" s="2">
+        <v>2063573</v>
+      </c>
+      <c r="C114" s="2">
+        <v>1994743</v>
+      </c>
+      <c r="D114" s="2">
+        <v>10899</v>
+      </c>
+      <c r="E114" s="2">
+        <v>4592</v>
+      </c>
+      <c r="F114" s="2">
+        <v>75902</v>
+      </c>
+      <c r="G114" s="2">
+        <v>50606</v>
+      </c>
+      <c r="H114" s="2">
+        <v>36029</v>
+      </c>
+      <c r="I114" s="2">
+        <v>2197</v>
+      </c>
+      <c r="J114" s="2">
+        <v>15113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>143</v>
+      </c>
+      <c r="B115" s="2">
+        <v>2032667</v>
+      </c>
+      <c r="C115" s="2">
+        <v>1965630</v>
+      </c>
+      <c r="D115" s="2">
+        <v>10532</v>
+      </c>
+      <c r="E115" s="2">
+        <v>4826</v>
+      </c>
+      <c r="F115" s="2">
+        <v>72371</v>
+      </c>
+      <c r="G115" s="2">
+        <v>47932</v>
+      </c>
+      <c r="H115" s="2">
+        <v>34256</v>
+      </c>
+      <c r="I115" s="2">
+        <v>2045</v>
+      </c>
+      <c r="J115" s="2">
+        <v>15378</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A529607B-4B94-40C1-A5CF-F43C3829DA97}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>